<commit_message>
Updated v1/welcome call to return UserDetail
</commit_message>
<xml_diff>
--- a/MoneyTracker/Helpers/Excel/SeedFiles/UserAccounts.xlsx
+++ b/MoneyTracker/Helpers/Excel/SeedFiles/UserAccounts.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmadhanlala\source\repos\nedbank-money-tracker\MoneyTracker\MoneyTracker\Helpers\Excel\SeedFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IQ\Projects\NedBank\Code\BitBucket\dev\nedbank-money-tracker\MoneyTracker\MoneyTracker\Helpers\Excel\SeedFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376440D7-8158-430F-B5CC-BEA3D6E9C24C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="2484" yWindow="2184" windowWidth="21600" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>UserAccountId</t>
   </si>
@@ -59,40 +60,58 @@
     <t>UserDetailId</t>
   </si>
   <si>
-    <t>UserDashboardAccountId</t>
-  </si>
-  <si>
     <t>Bank</t>
   </si>
   <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>KEYONA BUNDLE</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>Investment</t>
-  </si>
-  <si>
-    <t>Entrepreneur Fund R</t>
-  </si>
-  <si>
-    <t>INV</t>
-  </si>
-  <si>
-    <t>Beth</t>
-  </si>
-  <si>
-    <t>Danny</t>
+    <t>1066898235</t>
+  </si>
+  <si>
+    <t>1602334536</t>
+  </si>
+  <si>
+    <t>1633281132</t>
+  </si>
+  <si>
+    <t>4922130000784779</t>
+  </si>
+  <si>
+    <t>5898460761682640</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Savings Account </t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>Test User Welcome</t>
+  </si>
+  <si>
+    <t>Tom Savings</t>
+  </si>
+  <si>
+    <t>Beth Savings</t>
+  </si>
+  <si>
+    <t>Danny Savings</t>
+  </si>
+  <si>
+    <t>Test User Card</t>
+  </si>
+  <si>
+    <t>Beth Card</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -122,12 +141,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,11 +462,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,10 +480,9 @@
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,216 +510,199 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
-        <v>1108366655</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
+      <c r="B2" s="5">
+        <v>1066898235</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I2">
-        <v>11</v>
-      </c>
-      <c r="J2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
-        <v>4005455</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H3" t="s">
-        <v>16</v>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
       </c>
       <c r="I3">
         <v>11</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
-        <v>1108366652</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I4">
         <v>12</v>
       </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
-        <v>4005456</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>15</v>
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H5" t="s">
-        <v>16</v>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
       </c>
       <c r="I5">
         <v>13</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
-        <v>1108366659</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>12</v>
+      <c r="D6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I6">
-        <v>13</v>
-      </c>
-      <c r="J6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
-        <v>1108366651</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>12</v>
+      <c r="D7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="I7">
-        <v>13</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="3"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>